<commit_message>
remove .idea and cache files
</commit_message>
<xml_diff>
--- a/HTC_report.xlsx
+++ b/HTC_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>FACILITY</t>
   </si>
@@ -68,10 +68,16 @@
     <t>Chifunga Health Centre</t>
   </si>
   <si>
+    <t>✔</t>
+  </si>
+  <si>
     <t>Dambe Health Centre</t>
   </si>
   <si>
     <t>Ligowe Dispensary</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>Lisungwi Health Centre</t>
@@ -115,10 +121,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -160,11 +166,146 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -173,50 +314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -224,97 +321,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -325,25 +331,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,37 +463,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,115 +487,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,41 +601,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,6 +642,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -669,155 +681,149 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -830,14 +836,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1234,7 +1240,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54074074074074" defaultRowHeight="15"/>
@@ -1299,36 +1305,34 @@
         <v>320</v>
       </c>
       <c r="D2" s="4">
-        <v>329</v>
-      </c>
-      <c r="E2" s="6" t="str">
-        <f t="shared" ref="E2:E16" si="0">IF(D2&gt;=C2,"✔","X")</f>
-        <v>✔</v>
+        <v>344</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="4">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="4">
-        <v>2</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6" t="str">
-        <f t="shared" ref="I2:I16" si="1">IF(H2&gt;0,"X","✔")</f>
-        <v>✔</v>
-      </c>
-      <c r="J2" s="4">
-        <v>2</v>
-      </c>
-      <c r="K2" s="4">
-        <v>2</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
       <c r="M2" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N2" s="4">
         <v>0</v>
@@ -1336,27 +1340,24 @@
       <c r="O2" s="4">
         <v>0</v>
       </c>
-      <c r="P2" s="4">
-        <v>0</v>
-      </c>
+      <c r="P2" s="4"/>
       <c r="Q2">
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:17">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="4">
         <v>320</v>
       </c>
       <c r="D3" s="4">
-        <v>231</v>
-      </c>
-      <c r="E3" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
+        <v>320</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="4">
         <v>3</v>
@@ -1367,50 +1368,48 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I3" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="4">
         <v>3</v>
       </c>
       <c r="K3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="4">
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:17">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="4">
         <v>320</v>
       </c>
       <c r="D4" s="4">
-        <v>246</v>
-      </c>
-      <c r="E4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
+        <v>314</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -1421,9 +1420,8 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="4">
         <v>1</v>
@@ -1448,48 +1446,46 @@
       </c>
       <c r="Q4">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:17">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4">
         <v>480</v>
       </c>
       <c r="D5" s="4">
-        <v>406</v>
-      </c>
-      <c r="E5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
+        <v>513</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J5" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K5" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
@@ -1502,48 +1498,46 @@
       </c>
       <c r="Q5">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:17">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="4">
         <v>160</v>
       </c>
       <c r="D6" s="4">
-        <v>192</v>
-      </c>
-      <c r="E6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>151</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
       </c>
       <c r="M6" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N6" s="4">
         <v>0</v>
@@ -1556,45 +1550,43 @@
       </c>
       <c r="Q6">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:17">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="4">
         <v>160</v>
       </c>
       <c r="D7" s="4">
-        <v>159</v>
-      </c>
-      <c r="E7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
+        <v>100</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="4">
         <v>0</v>
@@ -1610,48 +1602,46 @@
       </c>
       <c r="Q7">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:17">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="4">
         <v>160</v>
       </c>
       <c r="D8" s="4">
-        <v>162</v>
-      </c>
-      <c r="E8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>160</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="4">
         <v>1</v>
       </c>
       <c r="M8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="4">
         <v>0</v>
@@ -1664,77 +1654,74 @@
       </c>
       <c r="Q8">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:17">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4">
         <v>320</v>
       </c>
       <c r="D9" s="4">
-        <v>346</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>411</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K9" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L9" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M9" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N9" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O9" s="4">
         <v>0</v>
       </c>
       <c r="P9" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:17">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
         <v>160</v>
       </c>
       <c r="D10" s="4">
-        <v>180</v>
-      </c>
-      <c r="E10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>165</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F10" s="4">
         <v>4</v>
@@ -1745,75 +1732,72 @@
       <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J10" s="4">
         <v>4</v>
       </c>
       <c r="K10" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N10" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10" s="4">
         <v>0</v>
       </c>
       <c r="P10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:17">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
         <v>640</v>
       </c>
       <c r="D11" s="4">
-        <v>951</v>
-      </c>
-      <c r="E11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>654</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F11" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="J11" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K11" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L11" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M11" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N11" s="4">
         <v>0</v>
@@ -1826,90 +1810,86 @@
       </c>
       <c r="Q11">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:17">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
         <v>160</v>
       </c>
       <c r="D12" s="4">
-        <v>169</v>
-      </c>
-      <c r="E12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>190</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="4">
         <v>1</v>
       </c>
       <c r="L12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="4">
         <v>0</v>
       </c>
       <c r="Q12">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:17">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="4">
         <v>160</v>
       </c>
       <c r="D13" s="4">
-        <v>165</v>
-      </c>
-      <c r="E13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>60</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F13" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H13" s="4">
         <v>0</v>
       </c>
-      <c r="I13" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J13" s="4">
         <v>0</v>
@@ -1934,48 +1914,46 @@
       </c>
       <c r="Q13">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:17">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4">
         <v>160</v>
       </c>
       <c r="D14" s="4">
-        <v>221</v>
-      </c>
-      <c r="E14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>176</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
       </c>
-      <c r="I14" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="4">
         <v>0</v>
       </c>
       <c r="M14" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="4">
         <v>0</v>
@@ -1988,77 +1966,74 @@
       </c>
       <c r="Q14">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:17">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="4">
         <v>320</v>
       </c>
       <c r="D15" s="4">
-        <v>437</v>
-      </c>
-      <c r="E15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>✔</v>
+        <v>491</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F15" s="4">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="4">
+        <v>11</v>
+      </c>
+      <c r="K15" s="4">
         <v>10</v>
       </c>
-      <c r="G15" s="4">
-        <v>9</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="J15" s="4">
-        <v>10</v>
-      </c>
-      <c r="K15" s="4">
-        <v>6</v>
-      </c>
       <c r="L15" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M15" s="4">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="N15" s="4">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="O15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="Q15">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:17">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="4">
         <v>160</v>
       </c>
       <c r="D16" s="4">
-        <v>50</v>
-      </c>
-      <c r="E16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
+        <v>42</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -2069,9 +2044,8 @@
       <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="I16" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>✔</v>
+      <c r="I16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -2096,7 +2070,7 @@
       </c>
       <c r="Q16">
         <f>$Q$2</f>
-        <v>202401</v>
+        <v>202308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>